<commit_message>
Corrigir Building Vite e Vercel
</commit_message>
<xml_diff>
--- a/public/formulario.xlsx
+++ b/public/formulario.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hugo\DPU\Projetos\novos\empresa-xyz\public\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899A1ECC-F7CD-4B07-AA1A-95B9DBDB81FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Admin" sheetId="1" r:id="rId1"/>
-    <sheet name="Perguntas1" sheetId="2" r:id="rId2"/>
-    <sheet name="Perguntas2" sheetId="3" r:id="rId3"/>
-    <sheet name="Perguntas3" sheetId="4" r:id="rId4"/>
-    <sheet name="Perguntas4" sheetId="5" r:id="rId5"/>
-    <sheet name="Perguntas5" sheetId="6" r:id="rId6"/>
+    <sheet name="Admin" sheetId="1" r:id="rId4"/>
+    <sheet name="Perguntas1" sheetId="2" r:id="rId5"/>
+    <sheet name="Perguntas2" sheetId="3" r:id="rId6"/>
+    <sheet name="Perguntas3" sheetId="4" r:id="rId7"/>
+    <sheet name="Perguntas4" sheetId="5" r:id="rId8"/>
+    <sheet name="Perguntas5" sheetId="6" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>IdUsuario</t>
   </si>
@@ -48,25 +43,25 @@
     <t>florangela.coelho</t>
   </si>
   <si>
+    <t>sdfsdf</t>
+  </si>
+  <si>
+    <t>hugo.dasilva</t>
+  </si>
+  <si>
+    <t>Uc04002@73</t>
+  </si>
+  <si>
+    <t>ssdfsfd</t>
+  </si>
+  <si>
+    <t>teste</t>
+  </si>
+  <si>
+    <t>teste 2</t>
+  </si>
+  <si>
     <t>respondente</t>
-  </si>
-  <si>
-    <t>sdfsdf</t>
-  </si>
-  <si>
-    <t>hugo.dasilva</t>
-  </si>
-  <si>
-    <t>Uc04002@73</t>
-  </si>
-  <si>
-    <t>ssdfsfd</t>
-  </si>
-  <si>
-    <t>teste</t>
-  </si>
-  <si>
-    <t>teste 2</t>
   </si>
   <si>
     <t>Você encontrou algum tipo de dificuldade ao navegar no portal da Empresa XYZ?</t>
@@ -117,23 +112,34 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="single"/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
@@ -176,25 +182,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -484,20 +482,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="true" style="0"/>
+    <col min="2" max="2" width="26.140625" customWidth="true" style="0"/>
+    <col min="3" max="3" width="26.140625" customWidth="true" style="0"/>
+    <col min="4" max="4" width="26.140625" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,7 +514,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>2</v>
       </c>
@@ -525,7 +528,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>3</v>
       </c>
@@ -539,12 +542,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -553,12 +556,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -567,26 +570,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -595,12 +598,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>6</v>
@@ -609,12 +612,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>9</v>
@@ -623,49 +626,102 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C6" r:id="rId_hyperlink_1"/>
   </hyperlinks>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="1" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" r:id="rId2ps"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="0" workbookViewId="0" zoomScale="160" zoomScaleNormal="160" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="82.7109375" customWidth="1"/>
-    <col min="3" max="3" width="53.85546875" customWidth="1"/>
-    <col min="4" max="4" width="61.140625" customWidth="1"/>
-    <col min="5" max="5" width="89.85546875" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="true" style="0"/>
+    <col min="2" max="2" width="82.7109375" customWidth="true" style="0"/>
+    <col min="3" max="3" width="53.85546875" customWidth="true" style="0"/>
+    <col min="4" max="4" width="61.140625" customWidth="true" style="0"/>
+    <col min="5" max="5" width="89.85546875" customWidth="true" style="0"/>
+    <col min="6" max="6" width="29.42578125" customWidth="true" style="0"/>
+    <col min="7" max="7" width="22.7109375" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -688,7 +744,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>2</v>
       </c>
@@ -705,7 +761,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>3</v>
       </c>
@@ -722,7 +778,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>4</v>
       </c>
@@ -739,7 +795,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>5</v>
       </c>
@@ -756,7 +812,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>6</v>
       </c>
@@ -773,7 +829,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>7</v>
       </c>
@@ -790,7 +846,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>8</v>
       </c>
@@ -807,7 +863,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>9</v>
       </c>
@@ -824,33 +880,47 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="0" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" showGridLines="true" showRowColHeaders="1" topLeftCell="C1">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="76.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="2" max="2" width="76.5703125" customWidth="true" style="0"/>
+    <col min="3" max="3" width="54.5703125" customWidth="true" style="0"/>
+    <col min="4" max="4" width="61.28515625" customWidth="true" style="0"/>
+    <col min="5" max="5" width="24" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -867,7 +937,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>2</v>
       </c>
@@ -881,7 +951,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>6</v>
       </c>
@@ -895,32 +965,46 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="78.140625" customWidth="1"/>
-    <col min="3" max="3" width="53.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="true" style="0"/>
+    <col min="2" max="2" width="78.140625" customWidth="true" style="0"/>
+    <col min="3" max="3" width="53.85546875" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -931,7 +1015,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -942,7 +1026,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>6</v>
       </c>
@@ -953,32 +1037,46 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="75.42578125" customWidth="1"/>
-    <col min="3" max="3" width="53.85546875" customWidth="1"/>
-    <col min="4" max="4" width="83.140625" customWidth="1"/>
+    <col min="2" max="2" width="75.42578125" customWidth="true" style="0"/>
+    <col min="3" max="3" width="53.85546875" customWidth="true" style="0"/>
+    <col min="4" max="4" width="83.140625" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -992,7 +1090,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1003,7 +1101,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>6</v>
       </c>
@@ -1014,32 +1112,46 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="81.7109375" customWidth="1"/>
-    <col min="3" max="3" width="100.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="true" style="0"/>
+    <col min="2" max="2" width="81.7109375" customWidth="true" style="0"/>
+    <col min="3" max="3" width="100.7109375" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1050,7 +1162,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1061,7 +1173,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>6</v>
       </c>
@@ -1072,12 +1184,23 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>